<commit_message>
added addPosition functionality to add more distinct rows
</commit_message>
<xml_diff>
--- a/documents/Professional growth.xlsx
+++ b/documents/Professional growth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Professional Growth Chart\professional-growth-chart\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Growth-chart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97199ED6-806A-411E-8545-C07F33C74CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C31854B-7D15-4330-A849-44136E6A730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Year</t>
   </si>
@@ -122,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +138,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -189,6 +213,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3459,7 +3487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA16C5F6-0A91-4094-B1CA-3CF42BB7C902}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -5564,10 +5592,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D4F916-7560-41A2-ADE7-C27181DBF36E}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:N15"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5703,6 +5731,174 @@
         <v>2050</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1">
+        <v>2020</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2021</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="1">
+        <v>20</v>
+      </c>
+      <c r="J15" s="1">
+        <v>22</v>
+      </c>
+      <c r="K15" s="1">
+        <v>27</v>
+      </c>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="1">
+        <v>10</v>
+      </c>
+      <c r="J16" s="1">
+        <v>22</v>
+      </c>
+      <c r="K16" s="1">
+        <v>21</v>
+      </c>
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H17" s="16"/>
+      <c r="I17" s="16">
+        <v>2020</v>
+      </c>
+      <c r="J17" s="16">
+        <v>2021</v>
+      </c>
+      <c r="K17" s="16">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="16">
+        <v>20</v>
+      </c>
+      <c r="J18" s="16">
+        <v>22</v>
+      </c>
+      <c r="K18" s="16">
+        <v>27</v>
+      </c>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="16">
+        <v>10</v>
+      </c>
+      <c r="J19" s="16">
+        <v>22</v>
+      </c>
+      <c r="K19" s="16">
+        <v>21</v>
+      </c>
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H20" s="17"/>
+      <c r="I20" s="17">
+        <v>2024</v>
+      </c>
+      <c r="J20" s="17">
+        <v>2025</v>
+      </c>
+      <c r="K20" s="17">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="17">
+        <v>20</v>
+      </c>
+      <c r="J21" s="17">
+        <v>22</v>
+      </c>
+      <c r="K21" s="17">
+        <v>27</v>
+      </c>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H22" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="17">
+        <v>10</v>
+      </c>
+      <c r="J22" s="17">
+        <v>22</v>
+      </c>
+      <c r="K22" s="17">
+        <v>21</v>
+      </c>
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H23" s="18"/>
+      <c r="I23" s="18">
+        <v>2020</v>
+      </c>
+      <c r="J23" s="18">
+        <v>2021</v>
+      </c>
+      <c r="K23" s="18">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="24" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H24" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="18">
+        <v>20</v>
+      </c>
+      <c r="J24" s="18">
+        <v>22</v>
+      </c>
+      <c r="K24" s="18">
+        <v>27</v>
+      </c>
+      <c r="L24" s="15"/>
+    </row>
+    <row r="25" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H25" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="18">
+        <v>10</v>
+      </c>
+      <c r="J25" s="18">
+        <v>22</v>
+      </c>
+      <c r="K25" s="18">
+        <v>21</v>
+      </c>
+      <c r="L25" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="I7:J7"/>

</xml_diff>